<commit_message>
aggiunta filigrana + firma
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/master_ridotta.xlsx
+++ b/Attestati Corsi di Formazione/master_ridotta.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>moodle_institution</t>
   </si>
@@ -81,9 +81,6 @@
     <t>TIVOLI</t>
   </si>
   <si>
-    <t>Percorso 1 - 27431 I SISTEMI INFORMATICI</t>
-  </si>
-  <si>
     <t>completo</t>
   </si>
   <si>
@@ -115,6 +112,30 @@
   </si>
   <si>
     <t>id_corso</t>
+  </si>
+  <si>
+    <t>FOOD &amp; DELIVERY</t>
+  </si>
+  <si>
+    <t>GIULIANI</t>
+  </si>
+  <si>
+    <t>ANNA</t>
+  </si>
+  <si>
+    <t>GLNNNA68D64H439I</t>
+  </si>
+  <si>
+    <t>14/15</t>
+  </si>
+  <si>
+    <t>02756840696</t>
+  </si>
+  <si>
+    <t>HACCP &amp; CELIACHIA 2025</t>
+  </si>
+  <si>
+    <t>petrignani</t>
   </si>
 </sst>
 </file>
@@ -351,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -423,12 +444,12 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -445,11 +466,9 @@
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2">
         <v>540</v>
@@ -458,22 +477,22 @@
         <v>540</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -481,26 +500,26 @@
     </row>
     <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4">
         <v>23743</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2">
         <v>540</v>
@@ -509,25 +528,74 @@
         <v>540</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4">
+        <v>24952</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2">
+        <v>300</v>
+      </c>
+      <c r="J4" s="2">
+        <v>300</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>